<commit_message>
Add command to run a Python script
--HG--
branch : dev
</commit_message>
<xml_diff>
--- a/doc/xcpshell-cmds.xlsx
+++ b/doc/xcpshell-cmds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Command</t>
   </si>
@@ -36,6 +36,21 @@
   </si>
   <si>
     <t>source &lt;filename&gt;</t>
+  </si>
+  <si>
+    <t>Commands are simply interpreted by the xcpshell.</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>Run python from a file</t>
+  </si>
+  <si>
+    <t>py &lt;filename&gt;</t>
+  </si>
+  <si>
+    <t>The shell object will be a global called 'shell' in the context of the Python script.</t>
   </si>
   <si>
     <t>interface</t>
@@ -359,10 +374,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -399,274 +414,290 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="D6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="0"/>
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="D19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="0"/>
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>